<commit_message>
Updated journey page with new layout
</commit_message>
<xml_diff>
--- a/public/journey.xlsx
+++ b/public/journey.xlsx
@@ -1,19 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29311"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29324"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\working\waccache\DB5PEPF0001176C\EXCELCNV\cbead8c1-c770-4b12-8d30-1cc641d9343c\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="52" documentId="8_{19D02D05-7873-4C33-9723-BB2DAAF55CC2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C4C40719-5F10-41B7-9BB1-864CABE19919}"/>
+  <xr:revisionPtr revIDLastSave="9" documentId="11_062041FF9FC8F54E906C5ECE42DE7EBF4E1D8E96" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{CDBF6718-F247-49F2-B73F-C5A1864896DD}"/>
   <bookViews>
     <workbookView xWindow="-60" yWindow="-60" windowWidth="15480" windowHeight="11640" xr2:uid="{8B30A10D-2D48-4ED4-AFDC-CE321B0E89B9}"/>
   </bookViews>
   <sheets>
-    <sheet name="in" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191028"/>
   <extLst>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="238" uniqueCount="143">
   <si>
     <t>title</t>
   </si>
@@ -53,12 +53,202 @@
     <t>role</t>
   </si>
   <si>
+    <t>6 Behavioral Nudges to Reduce Bias in Hiring and Promotions</t>
+  </si>
+  <si>
+    <t>Everyone who has worked to get diversity right knows there is no elixir that increases diverse talent in leadership roles. Doing DEI by the numbers just won’t get you there. But here’s some good news: By focusing on decision intelligence, and on evidence-based solutions that drive scalable change and increase inclusion, leaders can increase the number of diverse candidates that they hire and promote.</t>
+  </si>
+  <si>
+    <t>https://hbr.org/2022/11/6-behavioral-nudges-to-reduce-bias-in-hiring-and-promotions</t>
+  </si>
+  <si>
+    <t>HBR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">managers </t>
+  </si>
+  <si>
+    <t>How to reduce bias in your workplace</t>
+  </si>
+  <si>
+    <t>We all have bias -- especially the unconscious kind -- and it's preventing us from doing our best work. Gone unchecked, bias can make employees feel resentful, frustrated and silenced, and it can even lead to outright discrimination and harassment. Check out three key ways to reduce bias at work, according to Just Work cofounders Kim Scott and Trier Bryant.</t>
+  </si>
+  <si>
+    <t>https://www.ted.com/talks/kim_scott_and_trier_bryant_how_to_reduce_bias_in_your_workplace</t>
+  </si>
+  <si>
+    <t>TED Talks</t>
+  </si>
+  <si>
+    <t>A New Way to Combat Bias at Work</t>
+  </si>
+  <si>
+    <t>Joan Williams says that it's extremely difficult for organizations to rid their workforces of the unconscious biases that can prevent women and minorities from advancing. But it's not so hard for individual managers to interrupt bias within their own teams. She offers specific suggestions for how bosses can shift their approach in four areas: hiring, meetings, assignments, and reviews/promotions.</t>
+  </si>
+  <si>
+    <t>https://podcasts.apple.com/gb/podcast/a-new-way-to-combat-bias-at-work/id152022135?i=1000462472919</t>
+  </si>
+  <si>
+    <t>Podcast</t>
+  </si>
+  <si>
+    <t>What Makes an Inclusive Leader</t>
+  </si>
+  <si>
+    <t>Organizational leaders are increasingly leveraging inclusion to attract talent, retain employees, and motivate high creativity and excellence.</t>
+  </si>
+  <si>
+    <t>https://url.de.m.mimecastprotect.com/s/HKT_ClRZA6U9y6rZfq9qhK?domain=hbr.org</t>
+  </si>
+  <si>
+    <t>managers</t>
+  </si>
+  <si>
+    <t>Inclusive Leadership Training</t>
+  </si>
+  <si>
+    <t>iLearn</t>
+  </si>
+  <si>
+    <t>Belonging circles</t>
+  </si>
+  <si>
+    <t>What First-Time Managers Can Do to Address Burnout</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Becoming “the boss” is a significant career transition, and is often accompanied by shifting relationship dynamics at work, including leading direct reports. If managers don’t put their mental health first, burnout could easily rub off onto their teams. Here are some ways to take care of yourself as you start to lead.</t>
+  </si>
+  <si>
+    <t>https://hbr.org/2022/03/what-first-time-managers-can-do-to-address-burnout</t>
+  </si>
+  <si>
+    <t>Leading the 6-Generation Workforce</t>
+  </si>
+  <si>
+    <t>https://hbr.org/2024/04/leading-the-6-generation-workforce</t>
+  </si>
+  <si>
+    <t>12 top leaders share how they are redefining leadership to embrace inclusivity</t>
+  </si>
+  <si>
+    <t>As the next generation of leaders emerges and matures, it is imperative that we redefine leadership models to ensure they are inclusive and accessible to all. This article explores the emergence of this new leadership paradigm through the work of visionary Young Global Leaders who are championing change in various fields.</t>
+  </si>
+  <si>
+    <t>https://www.weforum.org/stories/2023/10/redefining-leadership-embracing-inclusivity-and-accessibility/</t>
+  </si>
+  <si>
+    <t>World Economic Forum</t>
+  </si>
+  <si>
+    <t>The Manager’s Guide to Inclusive Leadership — Small Habits That Make a Big Impact</t>
+  </si>
+  <si>
+    <t>https://review.firstround.com/the-managers-guide-to-inclusive-leadership-small-habits-that-make-a-big-impact/#why-the-%E2%80%9Ci%E2%80%9D-in-dei-matters-and-what-it-actually-means</t>
+  </si>
+  <si>
+    <t>Review</t>
+  </si>
+  <si>
+    <t>Are You Playing Favorites With Employee Recognition?</t>
+  </si>
+  <si>
+    <t>A common misconception shared by managers and leaders is that paychecks alone are enough to make employees feel valued. While paychecks are still important, real value is best conveyed by recognizing employees for who they are and what they do. Employee recognition engages, retains and develops employees.</t>
+  </si>
+  <si>
+    <t>https://www.gallup.com/workplace/392660/playing-favorites-employee-recognition.aspx</t>
+  </si>
+  <si>
+    <t>Gallup</t>
+  </si>
+  <si>
+    <t>Is Your Employee Recognition Really Authentic?</t>
+  </si>
+  <si>
+    <t>Employees want -- and need -- to be recognized at work for what they do and who they are. Gallup and Workhuman have uncovered many ways in which recognition boosts employees’ engagement, wellbeing, inclusion and belonging at work -- all of which may help to explain why organizations that make recognition a part of their culture also see cost-savings in retention.</t>
+  </si>
+  <si>
+    <t>https://www.gallup.com/workplace/508208/employee-recognition-really-authentic.aspx</t>
+  </si>
+  <si>
+    <t>It’s not about the office, it’s about belonging</t>
+  </si>
+  <si>
+    <t>To retain employees, organizations need to evolve their approach to building community, cohesion, and a sense of belonging at work.</t>
+  </si>
+  <si>
+    <t>https://www.mckinsey.com/capabilities/people-and-organizational-performance/our-insights/the-organization-blog/its-not-about-the-office-its-about-belonging</t>
+  </si>
+  <si>
+    <t>McKinsey&amp;Company</t>
+  </si>
+  <si>
+    <t>What Is Psychological Safety?</t>
+  </si>
+  <si>
+    <t>https://hbr.org/2023/02/what-is-psychological-safety</t>
+  </si>
+  <si>
+    <t>Diversity and Inclusion: Bottom-Up as Well as Top-Down</t>
+  </si>
+  <si>
+    <t>https://www.gallup.com/cliftonstrengths/en/266405/diversity-inclusion-bottom-top-down.aspx</t>
+  </si>
+  <si>
+    <t>Women in the Workplace 2024</t>
+  </si>
+  <si>
+    <t>Over the past decade, there have been important gains for women at every level of the corporate pipeline, particularly in senior leadership. Almost 30% of C-suite leaders are now women.
+However, the pipeline is not as healthy as the numbers suggest.</t>
+  </si>
+  <si>
+    <t>https://womenintheworkplace.com/</t>
+  </si>
+  <si>
+    <t>Report</t>
+  </si>
+  <si>
+    <t>Observatório da Discriminação Contra Pessoas LGBTI+</t>
+  </si>
+  <si>
+    <t>O Observatório da Discriminação Contra Pessoas LGBTI+ (lesbian, gay, bisexual, trans, intersex, and other identities) by ILGA Portugal is an online platform, available since 2013, aimed at receiving reports of discrimination and/or violence based on sexual orientation, gender identity and expression, or sexual characteristics occurring within Portuguese territory.</t>
+  </si>
+  <si>
+    <t>https://ilga-portugal.pt/denunciar-a-discriminacao/observatorio-da-discriminacao/</t>
+  </si>
+  <si>
+    <t>Global report on ageism</t>
+  </si>
+  <si>
+    <t>World Health Organization (2021). Global report on ageism. World Health Organization.</t>
+  </si>
+  <si>
+    <t>https://iris.who.int/items/5516b4d4-13bf-4fcd-82b3-2decd40164ee</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LGBTQIA+ </t>
+  </si>
+  <si>
+    <t>Don't Put People in Boxes</t>
+  </si>
+  <si>
+    <t>When we label people and put them in different boxes, we don't see PEOPLE for who they truly are.</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=zRwt25M5nGw</t>
+  </si>
+  <si>
+    <t>Video</t>
+  </si>
+  <si>
+    <t>hiring managers</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Gender </t>
+  </si>
+  <si>
     <t>Unlocking Belonging at Blip</t>
   </si>
   <si>
-    <t>iLearn</t>
-  </si>
-  <si>
     <t>everyone</t>
   </si>
   <si>
@@ -98,9 +288,6 @@
     <t>https://www.mckinsey.com/capabilities/people-and-organizational-performance/our-insights/why-diversity-matters</t>
   </si>
   <si>
-    <t>HBR</t>
-  </si>
-  <si>
     <t>Why DEI Still Matters (and How to Get It Right)</t>
   </si>
   <si>
@@ -128,9 +315,6 @@
     <t>https://www.ted.com/talks/carin_taylor_belonging_a_critical_piece_of_diversity_equity_inclusion</t>
   </si>
   <si>
-    <t>TED Talks</t>
-  </si>
-  <si>
     <t>Inclusion Unlocked</t>
   </si>
   <si>
@@ -140,9 +324,6 @@
     <t>https://open.spotify.com/show/4GYgaZyJgXJnlKLNrGZkLp</t>
   </si>
   <si>
-    <t>Podcast</t>
-  </si>
-  <si>
     <t>DEI After 5 with Sacha</t>
   </si>
   <si>
@@ -152,38 +333,146 @@
     <t>https://podcasts.apple.com/us/podcast/dei-after-5-with-sacha/id1723641701</t>
   </si>
   <si>
-    <t>What Makes an Inclusive Leader</t>
-  </si>
-  <si>
-    <t>Organizational leaders are increasingly leveraging inclusion to attract talent, retain employees, and motivate high creativity and excellence.</t>
-  </si>
-  <si>
-    <t>https://url.de.m.mimecastprotect.com/s/HKT_ClRZA6U9y6rZfq9qhK?domain=hbr.org</t>
-  </si>
-  <si>
-    <t>managers</t>
-  </si>
-  <si>
-    <t>Don't Put People in Boxes</t>
-  </si>
-  <si>
-    <t>When we label people and put them in different boxes, we don't see PEOPLE for who they truly are.</t>
-  </si>
-  <si>
-    <t>https://www.youtube.com/watch?v=zRwt25M5nGw</t>
-  </si>
-  <si>
-    <t>Video</t>
-  </si>
-  <si>
-    <t>hiring managers</t>
+    <t>The DEI Shift</t>
+  </si>
+  <si>
+    <t>Focusing on the healthcare sector, this podcast discusses DEI in medicine, offering practice-changing insights for healthcare professionals and leaders.​</t>
+  </si>
+  <si>
+    <t>https://open.spotify.com/show/12PUDntuHNwxZlEYftUFGH?si=c4f3aa43a24241c6</t>
+  </si>
+  <si>
+    <t>Living Corporate</t>
+  </si>
+  <si>
+    <t>A platform that amplifies Black and Brown voices in the workplace, providing authentic conversations about DEI and professional development.​</t>
+  </si>
+  <si>
+    <t>https://open.spotify.com/show/2mRmf9FpyH8GfhRNSQ1ZV9?si=cb32a36f3199406d</t>
+  </si>
+  <si>
+    <t>FinTech's DEI Discussions</t>
+  </si>
+  <si>
+    <t>This podcast delves into diversity, equity, and inclusion within the financial technology industry, featuring discussions with leaders driving change.​</t>
+  </si>
+  <si>
+    <t>https://open.spotify.com/show/0UHW1cPNqAouc2TaRga9ji?si=dfddd0b187cf452f</t>
+  </si>
+  <si>
+    <t>Diversity in Tech</t>
+  </si>
+  <si>
+    <t>The podcast that brings you expert advice and unique insights on diversity and inclusion in the tech industry. Whether you’re a software developer, a designer, a CTO, or a people manager, we’re here to help you make your workplace more accessible, open, and equitable.</t>
+  </si>
+  <si>
+    <t>https://open.spotify.com/show/0lAlYPM075iimuERRXuHM2?si=836681122b5b4b41</t>
+  </si>
+  <si>
+    <t>What DEI Gets Wrong — and How to Do It Right – Paolo Gaudiano</t>
+  </si>
+  <si>
+    <t>Discusses common misconceptions in DEI initiatives and offers data-driven approaches to implement meaningful change.​</t>
+  </si>
+  <si>
+    <t>https://www.ted.com/talks/paolo_gaudiano_what_dei_gets_wrong_and_how_to_do_it_right</t>
+  </si>
+  <si>
+    <t>We Need Leaders Who Boldly Champion Inclusion– June Sarpong</t>
+  </si>
+  <si>
+    <t>Calls for courageous leadership that actively promotes inclusion, arguing that such leadership is essential for organizational success.​</t>
+  </si>
+  <si>
+    <t>https://www.ted.com/talks/june_sarpong_we_need_leaders_who_boldly_champion_inclusion</t>
+  </si>
+  <si>
+    <t>How Diversity Makes Teams More Innovative – Rocío Lorenzo</t>
+  </si>
+  <si>
+    <t>Presents research demonstrating that diverse teams are more innovative, providing a compelling business case for diversity.​</t>
+  </si>
+  <si>
+    <t>https://www.ted.com/talks/rocio_lorenzo_how_diversity_makes_teams_more_innovative</t>
+  </si>
+  <si>
+    <t>Let's Stop Talking About Diversity and Start Working Towards Equity – Paloma Medina</t>
+  </si>
+  <si>
+    <t>Reframes the conversation from diversity to equity, advocating for systemic changes that promote fairness and inclusion.</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=deYUUfak08Y&amp;ab_channel=TEDxTalks</t>
+  </si>
+  <si>
+    <t>Humans are biased. Generative AI is even worse</t>
+  </si>
+  <si>
+    <t>Stable Diffusion’s text-to-image model amplifies stereotypes about race and gender — here’s why that matters.</t>
+  </si>
+  <si>
+    <t>https://www.bloomberg.com/graphics/2023-generative-ai-bias/</t>
+  </si>
+  <si>
+    <t>Bloomberg</t>
+  </si>
+  <si>
+    <t>Greater progress on diversity and inclusion essential to rebuild productive and resilient workplaces</t>
+  </si>
+  <si>
+    <t>High levels of diversity and inclusion in the workplace are associated with greater productivity, innovation and workforce well-being, yet too little is being done to promote them, particularly among minority groups, meaning that enterprises, workers and societies are missing out on considerable potential benefits.</t>
+  </si>
+  <si>
+    <t>https://www.ilo.org/resource/news/greater-progress-diversity-and-inclusion-essential-rebuild-productive-and</t>
+  </si>
+  <si>
+    <t>International Labour Organization</t>
+  </si>
+  <si>
+    <t>Diversity matters even more: The case for holistic impact</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Diversity Matters Even More is the fourth report in a McKinsey series investigating the business case for diversity, following Why Diversity Matters (2015), Delivering Through Diversity (2018), and Diversity Wins (2020). For almost a decade through our Diversity Matters series of reports, McKinsey has delivered a comprehensive global perspective on the relationship between leadership diversity and company performance. </t>
+  </si>
+  <si>
+    <t>https://www.mckinsey.com/featured-insights/diversity-and-inclusion/diversity-matters-even-more-the-case-for-holistic-impact</t>
+  </si>
+  <si>
+    <t>The Business Case For Diversity, Equity And Inclusion</t>
+  </si>
+  <si>
+    <t>Diversity, equity and inclusion have become critical components of business success. While these concepts are often viewed through the lens of social justice and morality, there is also a compelling business case for promoting diversity and creating a culture of inclusion in the workplace. From attracting top talent to fostering a more collaborative and creative workplace, the benefits of DEI are clear.</t>
+  </si>
+  <si>
+    <t>https://www.forbes.com/councils/forbesbusinessdevelopmentcouncil/2023/05/11/the-business-case-for-diversity-equity-and-inclusion/</t>
+  </si>
+  <si>
+    <t>Forbes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Age </t>
+  </si>
+  <si>
+    <t>Authoring Accessible Presentations in PowerPoint</t>
+  </si>
+  <si>
+    <t>This course offers an overview of practices and techniques you can use in Microsoft PowerPoint to author, and present accessibly and inclusively. You'll learn key concepts, explore built-in tools, and gain insights into how you can foster inclusivity.</t>
+  </si>
+  <si>
+    <t>https://rise.articulate.com/share/iabvEjEah94-kEGdR9yLCUKOvGPb7FJh#/</t>
+  </si>
+  <si>
+    <t>Guide</t>
+  </si>
+  <si>
+    <t>Accessibility</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="18">
+  <fonts count="20">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -318,6 +607,20 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="33">
     <fill>
@@ -616,7 +919,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="42">
+  <cellStyleXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
@@ -659,8 +962,9 @@
     <xf numFmtId="0" fontId="1" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -668,53 +972,60 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="42" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="42" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="42">
-    <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
-    <cellStyle name="20% - Accent2" xfId="23" builtinId="34" customBuiltin="1"/>
-    <cellStyle name="20% - Accent3" xfId="27" builtinId="38" customBuiltin="1"/>
-    <cellStyle name="20% - Accent4" xfId="31" builtinId="42" customBuiltin="1"/>
-    <cellStyle name="20% - Accent5" xfId="35" builtinId="46" customBuiltin="1"/>
-    <cellStyle name="20% - Accent6" xfId="39" builtinId="50" customBuiltin="1"/>
-    <cellStyle name="40% - Accent1" xfId="20" builtinId="31" customBuiltin="1"/>
-    <cellStyle name="40% - Accent2" xfId="24" builtinId="35" customBuiltin="1"/>
-    <cellStyle name="40% - Accent3" xfId="28" builtinId="39" customBuiltin="1"/>
-    <cellStyle name="40% - Accent4" xfId="32" builtinId="43" customBuiltin="1"/>
-    <cellStyle name="40% - Accent5" xfId="36" builtinId="47" customBuiltin="1"/>
-    <cellStyle name="40% - Accent6" xfId="40" builtinId="51" customBuiltin="1"/>
-    <cellStyle name="60% - Accent1" xfId="21" builtinId="32" customBuiltin="1"/>
-    <cellStyle name="60% - Accent2" xfId="25" builtinId="36" customBuiltin="1"/>
-    <cellStyle name="60% - Accent3" xfId="29" builtinId="40" customBuiltin="1"/>
-    <cellStyle name="60% - Accent4" xfId="33" builtinId="44" customBuiltin="1"/>
-    <cellStyle name="60% - Accent5" xfId="37" builtinId="48" customBuiltin="1"/>
-    <cellStyle name="60% - Accent6" xfId="41" builtinId="52" customBuiltin="1"/>
-    <cellStyle name="Accent1" xfId="18" builtinId="29" customBuiltin="1"/>
-    <cellStyle name="Accent2" xfId="22" builtinId="33" customBuiltin="1"/>
-    <cellStyle name="Accent3" xfId="26" builtinId="37" customBuiltin="1"/>
-    <cellStyle name="Accent4" xfId="30" builtinId="41" customBuiltin="1"/>
-    <cellStyle name="Accent5" xfId="34" builtinId="45" customBuiltin="1"/>
-    <cellStyle name="Accent6" xfId="38" builtinId="49" customBuiltin="1"/>
-    <cellStyle name="Bad" xfId="7" builtinId="27" customBuiltin="1"/>
-    <cellStyle name="Calculation" xfId="11" builtinId="22" customBuiltin="1"/>
-    <cellStyle name="Check Cell" xfId="13" builtinId="23" customBuiltin="1"/>
-    <cellStyle name="Explanatory Text" xfId="16" builtinId="53" customBuiltin="1"/>
-    <cellStyle name="Good" xfId="6" builtinId="26" customBuiltin="1"/>
-    <cellStyle name="Heading 1" xfId="2" builtinId="16" customBuiltin="1"/>
-    <cellStyle name="Heading 2" xfId="3" builtinId="17" customBuiltin="1"/>
-    <cellStyle name="Heading 3" xfId="4" builtinId="18" customBuiltin="1"/>
-    <cellStyle name="Heading 4" xfId="5" builtinId="19" customBuiltin="1"/>
-    <cellStyle name="Input" xfId="9" builtinId="20" customBuiltin="1"/>
-    <cellStyle name="Linked Cell" xfId="12" builtinId="24" customBuiltin="1"/>
-    <cellStyle name="Neutral" xfId="8" builtinId="28" customBuiltin="1"/>
+  <cellStyles count="43">
+    <cellStyle name="20% - Cor1" xfId="19" builtinId="30" customBuiltin="1"/>
+    <cellStyle name="20% - Cor2" xfId="23" builtinId="34" customBuiltin="1"/>
+    <cellStyle name="20% - Cor3" xfId="27" builtinId="38" customBuiltin="1"/>
+    <cellStyle name="20% - Cor4" xfId="31" builtinId="42" customBuiltin="1"/>
+    <cellStyle name="20% - Cor5" xfId="35" builtinId="46" customBuiltin="1"/>
+    <cellStyle name="20% - Cor6" xfId="39" builtinId="50" customBuiltin="1"/>
+    <cellStyle name="40% - Cor1" xfId="20" builtinId="31" customBuiltin="1"/>
+    <cellStyle name="40% - Cor2" xfId="24" builtinId="35" customBuiltin="1"/>
+    <cellStyle name="40% - Cor3" xfId="28" builtinId="39" customBuiltin="1"/>
+    <cellStyle name="40% - Cor4" xfId="32" builtinId="43" customBuiltin="1"/>
+    <cellStyle name="40% - Cor5" xfId="36" builtinId="47" customBuiltin="1"/>
+    <cellStyle name="40% - Cor6" xfId="40" builtinId="51" customBuiltin="1"/>
+    <cellStyle name="60% - Cor1" xfId="21" builtinId="32" customBuiltin="1"/>
+    <cellStyle name="60% - Cor2" xfId="25" builtinId="36" customBuiltin="1"/>
+    <cellStyle name="60% - Cor3" xfId="29" builtinId="40" customBuiltin="1"/>
+    <cellStyle name="60% - Cor4" xfId="33" builtinId="44" customBuiltin="1"/>
+    <cellStyle name="60% - Cor5" xfId="37" builtinId="48" customBuiltin="1"/>
+    <cellStyle name="60% - Cor6" xfId="41" builtinId="52" customBuiltin="1"/>
+    <cellStyle name="Cabeçalho 1" xfId="2" builtinId="16" customBuiltin="1"/>
+    <cellStyle name="Cabeçalho 2" xfId="3" builtinId="17" customBuiltin="1"/>
+    <cellStyle name="Cabeçalho 3" xfId="4" builtinId="18" customBuiltin="1"/>
+    <cellStyle name="Cabeçalho 4" xfId="5" builtinId="19" customBuiltin="1"/>
+    <cellStyle name="Cálculo" xfId="11" builtinId="22" customBuiltin="1"/>
+    <cellStyle name="Célula Ligada" xfId="12" builtinId="24" customBuiltin="1"/>
+    <cellStyle name="Cor1" xfId="18" builtinId="29" customBuiltin="1"/>
+    <cellStyle name="Cor2" xfId="22" builtinId="33" customBuiltin="1"/>
+    <cellStyle name="Cor3" xfId="26" builtinId="37" customBuiltin="1"/>
+    <cellStyle name="Cor4" xfId="30" builtinId="41" customBuiltin="1"/>
+    <cellStyle name="Cor5" xfId="34" builtinId="45" customBuiltin="1"/>
+    <cellStyle name="Cor6" xfId="38" builtinId="49" customBuiltin="1"/>
+    <cellStyle name="Correto" xfId="6" builtinId="26" customBuiltin="1"/>
+    <cellStyle name="Entrada" xfId="9" builtinId="20" customBuiltin="1"/>
+    <cellStyle name="Hyperlink" xfId="42" xr:uid="{00000000-000B-0000-0000-000008000000}"/>
+    <cellStyle name="Incorreto" xfId="7" builtinId="27" customBuiltin="1"/>
+    <cellStyle name="Neutro" xfId="8" builtinId="28" customBuiltin="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Note" xfId="15" builtinId="10" customBuiltin="1"/>
-    <cellStyle name="Output" xfId="10" builtinId="21" customBuiltin="1"/>
-    <cellStyle name="Title" xfId="1" builtinId="15" customBuiltin="1"/>
+    <cellStyle name="Nota" xfId="15" builtinId="10" customBuiltin="1"/>
+    <cellStyle name="Saída" xfId="10" builtinId="21" customBuiltin="1"/>
+    <cellStyle name="Texto de Aviso" xfId="14" builtinId="11" customBuiltin="1"/>
+    <cellStyle name="Texto Explicativo" xfId="16" builtinId="53" customBuiltin="1"/>
+    <cellStyle name="Título" xfId="1" builtinId="15" customBuiltin="1"/>
     <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
-    <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
+    <cellStyle name="Verificar Célula" xfId="13" builtinId="23" customBuiltin="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1026,18 +1337,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5CA93658-3BFB-40A3-9A82-CBFF82FF34B9}">
-  <dimension ref="A1:E13"/>
+  <dimension ref="A1:E50"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" topLeftCell="A42" workbookViewId="0">
+      <selection activeCell="E50" sqref="E50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="39.85546875" style="2" customWidth="1"/>
+    <col min="1" max="1" width="42.7109375" style="2" customWidth="1"/>
     <col min="2" max="2" width="94" style="2" customWidth="1"/>
     <col min="3" max="3" width="64.85546875" style="1" customWidth="1"/>
-    <col min="4" max="4" width="16.28515625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="25" style="1" customWidth="1"/>
     <col min="5" max="5" width="19.7109375" style="1" customWidth="1"/>
     <col min="6" max="16384" width="9.140625" style="1"/>
   </cols>
@@ -1059,201 +1370,847 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:5" ht="60.75">
       <c r="A2" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="2"/>
+      <c r="B2" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>7</v>
+      </c>
       <c r="D2" s="2" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="60.75">
       <c r="A3" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="60.75">
+      <c r="A4" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="30.75">
+      <c r="A5" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="D5" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C3" s="2"/>
-      <c r="D3" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" ht="30.75">
-      <c r="A4" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="E4" s="2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5">
-      <c r="A5" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>13</v>
-      </c>
       <c r="E5" s="2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" ht="30.75">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5">
       <c r="A6" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="E6" s="2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" ht="30.75">
+        <v>22</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5">
       <c r="A7" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="E7" s="1" t="s">
         <v>21</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="D7" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="E7" s="2" t="s">
-        <v>7</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="45.75">
       <c r="A8" s="2" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="C8" s="2" t="s">
         <v>26</v>
       </c>
+      <c r="C8" s="3" t="s">
+        <v>27</v>
+      </c>
       <c r="D8" s="2" t="s">
-        <v>20</v>
+        <v>8</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" ht="30.75">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5">
       <c r="A9" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="B9" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="C9" s="2" t="s">
+      <c r="B9" s="4"/>
+      <c r="C9" s="3" t="s">
         <v>29</v>
       </c>
       <c r="D9" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="60.75">
+      <c r="A10" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="E9" s="2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" ht="30.75">
-      <c r="A10" s="2" t="s">
+      <c r="B10" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="B10" s="2" t="s">
+      <c r="C10" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="C10" s="2" t="s">
+      <c r="D10" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="D10" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="E10" s="2" t="s">
-        <v>7</v>
+      <c r="E10" s="1" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="30.75">
       <c r="A11" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="C11" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="B11" s="2" t="s">
+      <c r="D11" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="C11" s="3" t="s">
+      <c r="E11" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" ht="60.75">
+      <c r="A12" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="D11" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="E11" s="2" t="s">
+      <c r="B12" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" ht="60.75">
+      <c r="A13" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" ht="45.75">
+      <c r="A14" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="C14" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5">
+      <c r="A15" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E15" s="2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" ht="30.75">
+      <c r="A16" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" ht="45.75">
+      <c r="A17" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="C17" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" ht="60.75">
+      <c r="A18" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="C18" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="E18" s="2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5">
+      <c r="A19" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="C19" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="E19" s="2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" ht="60.75">
+      <c r="A20" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="C20" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="E20" s="2" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5">
+      <c r="A21" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="D21" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="E21" s="2" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" ht="60.75">
+      <c r="A22" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C22" s="3" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="12" spans="1:5" ht="30.75">
-      <c r="A12" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="B12" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="C12" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="D12" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="E12" s="2" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5">
-      <c r="A13" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="B13" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="C13" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="D13" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="E13" s="2" t="s">
-        <v>46</v>
+      <c r="D22" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E22" s="2" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" ht="60.75">
+      <c r="A23" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C23" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D23" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E23" s="2" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" ht="60.75">
+      <c r="A24" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C24" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D24" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="E24" s="2" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" ht="45.75">
+      <c r="A25" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="C25" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="D25" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="E25" s="1" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5">
+      <c r="A26" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="C26" s="2"/>
+      <c r="D26" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="E26" s="2" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5">
+      <c r="A27" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="C27" s="2"/>
+      <c r="D27" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="E27" s="2" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" ht="30.75">
+      <c r="A28" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="B28" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="C28" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="D28" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="E28" s="2" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5">
+      <c r="A29" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="B29" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="C29" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="D29" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="E29" s="2" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" ht="30.75">
+      <c r="A30" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="B30" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="C30" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="D30" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E30" s="2" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" ht="30.75">
+      <c r="A31" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="B31" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="C31" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="D31" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E31" s="2" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" ht="45.75">
+      <c r="A32" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="B32" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="C32" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="D32" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E32" s="2" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" ht="30.75">
+      <c r="A33" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="B33" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="C33" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="D33" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E33" s="2" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" ht="30.75">
+      <c r="A34" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="B34" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="C34" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="D34" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="E34" s="2" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" ht="30.75">
+      <c r="A35" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="B35" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="C35" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="D35" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="E35" s="2" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" ht="30.75">
+      <c r="A36" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="B36" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="C36" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="D36" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="E36" s="2" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" ht="30.75">
+      <c r="A37" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="B37" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="C37" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="D37" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="E37" s="2" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" ht="30.75">
+      <c r="A38" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="B38" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="C38" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="D38" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="E38" s="2" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" ht="45.75">
+      <c r="A39" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="B39" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="C39" s="3" t="s">
+        <v>109</v>
+      </c>
+      <c r="D39" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="E39" s="2" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" ht="30.75">
+      <c r="A40" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="B40" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="C40" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="D40" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E40" s="2" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" ht="30.75">
+      <c r="A41" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="B41" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="C41" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="D41" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E41" s="2" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" ht="30.75">
+      <c r="A42" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="B42" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="C42" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="D42" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E42" s="2" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" ht="30.75">
+      <c r="A43" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="B43" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="C43" s="3" t="s">
+        <v>121</v>
+      </c>
+      <c r="D43" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E43" s="2" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" ht="30.75">
+      <c r="A44" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="B44" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="C44" s="3" t="s">
+        <v>124</v>
+      </c>
+      <c r="D44" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="E44" s="2" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" ht="60.75">
+      <c r="A45" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B45" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C45" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D45" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="E45" s="2" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" ht="45.75">
+      <c r="A46" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="B46" s="2" t="s">
+        <v>127</v>
+      </c>
+      <c r="C46" s="3" t="s">
+        <v>128</v>
+      </c>
+      <c r="D46" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="E46" s="1" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" ht="76.5">
+      <c r="A47" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="B47" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="C47" s="3" t="s">
+        <v>132</v>
+      </c>
+      <c r="D47" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="E47" s="1" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" ht="60.75">
+      <c r="A48" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="B48" s="2" t="s">
+        <v>134</v>
+      </c>
+      <c r="C48" s="3" t="s">
+        <v>135</v>
+      </c>
+      <c r="D48" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="E48" s="1" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5">
+      <c r="A49" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="B49" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="C49" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="D49" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="E49" s="2" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" ht="45.75">
+      <c r="A50" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="B50" s="2" t="s">
+        <v>139</v>
+      </c>
+      <c r="C50" s="3" t="s">
+        <v>140</v>
+      </c>
+      <c r="D50" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="E50" s="1" t="s">
+        <v>142</v>
       </c>
     </row>
   </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E49">
+    <sortCondition descending="1" ref="E2:E49"/>
+  </sortState>
+  <hyperlinks>
+    <hyperlink ref="C36" r:id="rId1" xr:uid="{08FDF4D0-7481-4C65-9F6E-C8F9B5F72231}"/>
+    <hyperlink ref="C37" r:id="rId2" xr:uid="{1DD9AF47-DA73-48A1-A84C-454BF0B34B70}"/>
+    <hyperlink ref="C39" r:id="rId3" xr:uid="{956EA655-5BF0-425F-A535-934F04C171A8}"/>
+    <hyperlink ref="C38" r:id="rId4" xr:uid="{4E644E3D-5CB9-488A-9ACB-C705A4341945}"/>
+    <hyperlink ref="C41" r:id="rId5" xr:uid="{6C86356C-E1E7-4E6C-913B-1397244ECB0A}"/>
+    <hyperlink ref="C40" r:id="rId6" xr:uid="{23A3154D-09FE-45BD-AF3F-4B6A7F4A981C}"/>
+    <hyperlink ref="C42" r:id="rId7" xr:uid="{FE6AF7A2-6B55-439A-A29B-2CAEAFA1A8D3}"/>
+    <hyperlink ref="C43" r:id="rId8" xr:uid="{B640DEDD-DE10-43AB-8D82-A39FEBA876E6}"/>
+    <hyperlink ref="C44" r:id="rId9" xr:uid="{C0FD5840-93DC-4F1A-B75A-89DF24EB40E8}"/>
+    <hyperlink ref="C8" r:id="rId10" xr:uid="{425FB193-8FFE-4108-B2C9-8BC3634B344D}"/>
+    <hyperlink ref="C9" r:id="rId11" xr:uid="{6B4D7D83-FF82-4423-B9FA-60CC3D1B7599}"/>
+    <hyperlink ref="C10" r:id="rId12" xr:uid="{4603BF52-AFF1-4399-B92A-413883430FEA}"/>
+    <hyperlink ref="C11" r:id="rId13" location="why-the-%E2%80%9Ci%E2%80%9D-in-dei-matters-and-what-it-actually-means" xr:uid="{CB66CD6A-A2B0-4716-9521-08FCD0D9D404}"/>
+    <hyperlink ref="C12" r:id="rId14" xr:uid="{4C8700BE-95BB-4758-8FC1-08D058B8FC6D}"/>
+    <hyperlink ref="C13" r:id="rId15" xr:uid="{886808D6-D569-42AD-B714-7C59EFA3DDE3}"/>
+    <hyperlink ref="C14" r:id="rId16" xr:uid="{994801DC-2783-447E-B0AA-71BF9FEF8085}"/>
+    <hyperlink ref="C15" r:id="rId17" xr:uid="{52C82B08-BD86-46FB-8E30-D8C976F271F7}"/>
+    <hyperlink ref="C16" r:id="rId18" xr:uid="{AE603C53-48EC-4C2B-863C-2D8EA779ABA3}"/>
+    <hyperlink ref="C25" r:id="rId19" xr:uid="{8B612EBD-70F9-4CA6-BCC5-8B3773D19932}"/>
+    <hyperlink ref="C18" r:id="rId20" xr:uid="{5E30FE36-92B2-4FB5-B22E-12AFB2A19644}"/>
+    <hyperlink ref="C19" r:id="rId21" xr:uid="{99478175-8835-41F3-80FC-68E464C06143}"/>
+    <hyperlink ref="C2" r:id="rId22" xr:uid="{D56206BC-6E06-4AE1-A713-4F805E6C1479}"/>
+    <hyperlink ref="C3" r:id="rId23" xr:uid="{4E3B6E6B-DC59-4365-B28A-0AD888A824DE}"/>
+    <hyperlink ref="C4" r:id="rId24" xr:uid="{F78FBFC5-057A-496E-A6CB-D5F0F3CCB3F3}"/>
+    <hyperlink ref="C46" r:id="rId25" xr:uid="{6933C4BC-C0D3-4A9E-BB76-EC94C8B169B4}"/>
+    <hyperlink ref="C47" r:id="rId26" xr:uid="{AE1BE1E8-0323-4C66-9FFB-2D0C402FCFED}"/>
+    <hyperlink ref="C48" r:id="rId27" xr:uid="{D76B74D2-B0C0-4E71-92EF-5508BC637EE9}"/>
+    <hyperlink ref="C17" r:id="rId28" xr:uid="{144E4E4E-71FA-4D6E-8D76-2DB77CCCAD0F}"/>
+    <hyperlink ref="C20" r:id="rId29" xr:uid="{83C086BF-243D-4301-B05C-9550209C41DE}"/>
+    <hyperlink ref="C49" r:id="rId30" xr:uid="{79B8C40B-E249-4EF8-B7E9-457073A27692}"/>
+    <hyperlink ref="C22" r:id="rId31" xr:uid="{254E40CD-3A87-419C-8216-72AEDB747AF1}"/>
+    <hyperlink ref="C23" r:id="rId32" xr:uid="{69070A19-CC37-407E-9989-E9D213AD78C5}"/>
+    <hyperlink ref="C24" r:id="rId33" xr:uid="{BDDABA00-3BBF-47CC-901F-53692F5F4BE8}"/>
+    <hyperlink ref="C45" r:id="rId34" xr:uid="{397F1BF4-4E90-4516-B5E6-F02C14DD6256}"/>
+    <hyperlink ref="C50" r:id="rId35" location="/" xr:uid="{148ABF7C-1E6C-4BDD-B1E3-DC7183537F2D}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -1271,15 +2228,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101002A271A3A3D7AF442877022B0C11C9687" ma:contentTypeVersion="16" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="63fa5801969ef1641dc8e48b23697405">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="e5e4058b-80d7-4dc7-8f2f-eb1c13aca2ca" xmlns:ns3="c6ba0e2c-e3e3-40fb-b5f4-f2b39b1adc73" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="f82b11606e87c9a8efd2c68f403f8c59" ns2:_="" ns3:_="">
     <xsd:import namespace="e5e4058b-80d7-4dc7-8f2f-eb1c13aca2ca"/>
@@ -1522,14 +2470,23 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5F7C28EA-775F-4F37-B72F-351A20180A9E}"/>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{654B2479-4C14-46B2-AA03-90FA86AD05EA}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9829FA3B-CFB5-4FEC-A4DC-D57D48BF73C4}"/>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9829FA3B-CFB5-4FEC-A4DC-D57D48BF73C4}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{654B2479-4C14-46B2-AA03-90FA86AD05EA}"/>
 </file>
</xml_diff>

<commit_message>
Updated playlist automation with inactive items (excluding large video files)
</commit_message>
<xml_diff>
--- a/public/journey.xlsx
+++ b/public/journey.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29324"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29325"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\working\waccache\DB5PEPF0001176C\EXCELCNV\cbead8c1-c770-4b12-8d30-1cc641d9343c\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="9" documentId="11_062041FF9FC8F54E906C5ECE42DE7EBF4E1D8E96" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{CDBF6718-F247-49F2-B73F-C5A1864896DD}"/>
+  <xr:revisionPtr revIDLastSave="22" documentId="11_062041FF9FC8F54E906C5ECE42DE7EBF4E1D8E96" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{254C40FB-640C-4B62-B5A3-ED98065CCFAC}"/>
   <bookViews>
     <workbookView xWindow="-60" yWindow="-60" windowWidth="15480" windowHeight="11640" xr2:uid="{8B30A10D-2D48-4ED4-AFDC-CE321B0E89B9}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Folha1" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191028"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="238" uniqueCount="143">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="243" uniqueCount="141">
   <si>
     <t>title</t>
   </si>
@@ -249,15 +250,15 @@
     <t>Unlocking Belonging at Blip</t>
   </si>
   <si>
+    <t>Courses</t>
+  </si>
+  <si>
     <t>everyone</t>
   </si>
   <si>
     <t>Trailliant Self-paced Training</t>
   </si>
   <si>
-    <t>FlutterBe</t>
-  </si>
-  <si>
     <t>Diversity, Equity, and Inclusion: a Beginner's Guide</t>
   </si>
   <si>
@@ -267,9 +268,6 @@
     <t>https://ppb.udemy.com/course/diversity-equity-and-inclusion-a-beginners-guide/</t>
   </si>
   <si>
-    <t>Udemy</t>
-  </si>
-  <si>
     <t>Diversity And Inclusion In The Workplace</t>
   </si>
   <si>
@@ -288,6 +286,9 @@
     <t>https://www.mckinsey.com/capabilities/people-and-organizational-performance/our-insights/why-diversity-matters</t>
   </si>
   <si>
+    <t>Article</t>
+  </si>
+  <si>
     <t>Why DEI Still Matters (and How to Get It Right)</t>
   </si>
   <si>
@@ -303,7 +304,7 @@
     <t>Eight Powerful Truths.</t>
   </si>
   <si>
-    <t>https://www.deloitte.com/content/dam/insights/articles/2024/4209_diversity-and-inclusion-revolution/di-diversity-and-inclusion-revolution.pdf</t>
+    <t>https://www.deloitte.com/content/dam/insights/Article/2024/4209_diversity-and-inclusion-revolution/di-diversity-and-inclusion-revolution.pdf</t>
   </si>
   <si>
     <t>A Critical Piece of Diversity, Equity &amp; Inclusion - Carin Taylor</t>
@@ -414,9 +415,6 @@
     <t>https://www.bloomberg.com/graphics/2023-generative-ai-bias/</t>
   </si>
   <si>
-    <t>Bloomberg</t>
-  </si>
-  <si>
     <t>Greater progress on diversity and inclusion essential to rebuild productive and resilient workplaces</t>
   </si>
   <si>
@@ -445,9 +443,6 @@
   </si>
   <si>
     <t>https://www.forbes.com/councils/forbesbusinessdevelopmentcouncil/2023/05/11/the-business-case-for-diversity-equity-and-inclusion/</t>
-  </si>
-  <si>
-    <t>Forbes</t>
   </si>
   <si>
     <t xml:space="preserve">Age </t>
@@ -983,49 +978,49 @@
     </xf>
   </cellXfs>
   <cellStyles count="43">
-    <cellStyle name="20% - Cor1" xfId="19" builtinId="30" customBuiltin="1"/>
-    <cellStyle name="20% - Cor2" xfId="23" builtinId="34" customBuiltin="1"/>
-    <cellStyle name="20% - Cor3" xfId="27" builtinId="38" customBuiltin="1"/>
-    <cellStyle name="20% - Cor4" xfId="31" builtinId="42" customBuiltin="1"/>
-    <cellStyle name="20% - Cor5" xfId="35" builtinId="46" customBuiltin="1"/>
-    <cellStyle name="20% - Cor6" xfId="39" builtinId="50" customBuiltin="1"/>
-    <cellStyle name="40% - Cor1" xfId="20" builtinId="31" customBuiltin="1"/>
-    <cellStyle name="40% - Cor2" xfId="24" builtinId="35" customBuiltin="1"/>
-    <cellStyle name="40% - Cor3" xfId="28" builtinId="39" customBuiltin="1"/>
-    <cellStyle name="40% - Cor4" xfId="32" builtinId="43" customBuiltin="1"/>
-    <cellStyle name="40% - Cor5" xfId="36" builtinId="47" customBuiltin="1"/>
-    <cellStyle name="40% - Cor6" xfId="40" builtinId="51" customBuiltin="1"/>
-    <cellStyle name="60% - Cor1" xfId="21" builtinId="32" customBuiltin="1"/>
-    <cellStyle name="60% - Cor2" xfId="25" builtinId="36" customBuiltin="1"/>
-    <cellStyle name="60% - Cor3" xfId="29" builtinId="40" customBuiltin="1"/>
-    <cellStyle name="60% - Cor4" xfId="33" builtinId="44" customBuiltin="1"/>
-    <cellStyle name="60% - Cor5" xfId="37" builtinId="48" customBuiltin="1"/>
-    <cellStyle name="60% - Cor6" xfId="41" builtinId="52" customBuiltin="1"/>
-    <cellStyle name="Cabeçalho 1" xfId="2" builtinId="16" customBuiltin="1"/>
-    <cellStyle name="Cabeçalho 2" xfId="3" builtinId="17" customBuiltin="1"/>
-    <cellStyle name="Cabeçalho 3" xfId="4" builtinId="18" customBuiltin="1"/>
-    <cellStyle name="Cabeçalho 4" xfId="5" builtinId="19" customBuiltin="1"/>
-    <cellStyle name="Cálculo" xfId="11" builtinId="22" customBuiltin="1"/>
-    <cellStyle name="Célula Ligada" xfId="12" builtinId="24" customBuiltin="1"/>
-    <cellStyle name="Cor1" xfId="18" builtinId="29" customBuiltin="1"/>
-    <cellStyle name="Cor2" xfId="22" builtinId="33" customBuiltin="1"/>
-    <cellStyle name="Cor3" xfId="26" builtinId="37" customBuiltin="1"/>
-    <cellStyle name="Cor4" xfId="30" builtinId="41" customBuiltin="1"/>
-    <cellStyle name="Cor5" xfId="34" builtinId="45" customBuiltin="1"/>
-    <cellStyle name="Cor6" xfId="38" builtinId="49" customBuiltin="1"/>
-    <cellStyle name="Correto" xfId="6" builtinId="26" customBuiltin="1"/>
-    <cellStyle name="Entrada" xfId="9" builtinId="20" customBuiltin="1"/>
+    <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
+    <cellStyle name="20% - Accent2" xfId="23" builtinId="34" customBuiltin="1"/>
+    <cellStyle name="20% - Accent3" xfId="27" builtinId="38" customBuiltin="1"/>
+    <cellStyle name="20% - Accent4" xfId="31" builtinId="42" customBuiltin="1"/>
+    <cellStyle name="20% - Accent5" xfId="35" builtinId="46" customBuiltin="1"/>
+    <cellStyle name="20% - Accent6" xfId="39" builtinId="50" customBuiltin="1"/>
+    <cellStyle name="40% - Accent1" xfId="20" builtinId="31" customBuiltin="1"/>
+    <cellStyle name="40% - Accent2" xfId="24" builtinId="35" customBuiltin="1"/>
+    <cellStyle name="40% - Accent3" xfId="28" builtinId="39" customBuiltin="1"/>
+    <cellStyle name="40% - Accent4" xfId="32" builtinId="43" customBuiltin="1"/>
+    <cellStyle name="40% - Accent5" xfId="36" builtinId="47" customBuiltin="1"/>
+    <cellStyle name="40% - Accent6" xfId="40" builtinId="51" customBuiltin="1"/>
+    <cellStyle name="60% - Accent1" xfId="21" builtinId="32" customBuiltin="1"/>
+    <cellStyle name="60% - Accent2" xfId="25" builtinId="36" customBuiltin="1"/>
+    <cellStyle name="60% - Accent3" xfId="29" builtinId="40" customBuiltin="1"/>
+    <cellStyle name="60% - Accent4" xfId="33" builtinId="44" customBuiltin="1"/>
+    <cellStyle name="60% - Accent5" xfId="37" builtinId="48" customBuiltin="1"/>
+    <cellStyle name="60% - Accent6" xfId="41" builtinId="52" customBuiltin="1"/>
+    <cellStyle name="Accent1" xfId="18" builtinId="29" customBuiltin="1"/>
+    <cellStyle name="Accent2" xfId="22" builtinId="33" customBuiltin="1"/>
+    <cellStyle name="Accent3" xfId="26" builtinId="37" customBuiltin="1"/>
+    <cellStyle name="Accent4" xfId="30" builtinId="41" customBuiltin="1"/>
+    <cellStyle name="Accent5" xfId="34" builtinId="45" customBuiltin="1"/>
+    <cellStyle name="Accent6" xfId="38" builtinId="49" customBuiltin="1"/>
+    <cellStyle name="Bad" xfId="7" builtinId="27" customBuiltin="1"/>
+    <cellStyle name="Calculation" xfId="11" builtinId="22" customBuiltin="1"/>
+    <cellStyle name="Check Cell" xfId="13" builtinId="23" customBuiltin="1"/>
+    <cellStyle name="Explanatory Text" xfId="16" builtinId="53" customBuiltin="1"/>
+    <cellStyle name="Good" xfId="6" builtinId="26" customBuiltin="1"/>
+    <cellStyle name="Heading 1" xfId="2" builtinId="16" customBuiltin="1"/>
+    <cellStyle name="Heading 2" xfId="3" builtinId="17" customBuiltin="1"/>
+    <cellStyle name="Heading 3" xfId="4" builtinId="18" customBuiltin="1"/>
+    <cellStyle name="Heading 4" xfId="5" builtinId="19" customBuiltin="1"/>
     <cellStyle name="Hyperlink" xfId="42" xr:uid="{00000000-000B-0000-0000-000008000000}"/>
-    <cellStyle name="Incorreto" xfId="7" builtinId="27" customBuiltin="1"/>
-    <cellStyle name="Neutro" xfId="8" builtinId="28" customBuiltin="1"/>
+    <cellStyle name="Input" xfId="9" builtinId="20" customBuiltin="1"/>
+    <cellStyle name="Linked Cell" xfId="12" builtinId="24" customBuiltin="1"/>
+    <cellStyle name="Neutral" xfId="8" builtinId="28" customBuiltin="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Nota" xfId="15" builtinId="10" customBuiltin="1"/>
-    <cellStyle name="Saída" xfId="10" builtinId="21" customBuiltin="1"/>
-    <cellStyle name="Texto de Aviso" xfId="14" builtinId="11" customBuiltin="1"/>
-    <cellStyle name="Texto Explicativo" xfId="16" builtinId="53" customBuiltin="1"/>
-    <cellStyle name="Título" xfId="1" builtinId="15" customBuiltin="1"/>
+    <cellStyle name="Note" xfId="15" builtinId="10" customBuiltin="1"/>
+    <cellStyle name="Output" xfId="10" builtinId="21" customBuiltin="1"/>
+    <cellStyle name="Title" xfId="1" builtinId="15" customBuiltin="1"/>
     <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
-    <cellStyle name="Verificar Célula" xfId="13" builtinId="23" customBuiltin="1"/>
+    <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1339,8 +1334,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5CA93658-3BFB-40A3-9A82-CBFF82FF34B9}">
   <dimension ref="A1:E50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A42" workbookViewId="0">
-      <selection activeCell="E50" sqref="E50"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="D29" sqref="D29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1761,22 +1756,22 @@
       </c>
       <c r="C26" s="2"/>
       <c r="D26" s="2" t="s">
-        <v>23</v>
+        <v>70</v>
       </c>
       <c r="E26" s="2" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
     </row>
     <row r="27" spans="1:5">
       <c r="A27" s="2" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="C27" s="2"/>
       <c r="D27" s="2" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="E27" s="2" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
     </row>
     <row r="28" spans="1:5" ht="30.75">
@@ -1790,44 +1785,44 @@
         <v>75</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="E28" s="2" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
     </row>
     <row r="29" spans="1:5">
       <c r="A29" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="B29" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="B29" s="2" t="s">
+      <c r="C29" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="C29" s="2" t="s">
-        <v>79</v>
-      </c>
       <c r="D29" s="2" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="E29" s="2" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
     </row>
     <row r="30" spans="1:5" ht="30.75">
       <c r="A30" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="B30" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="B30" s="2" t="s">
+      <c r="C30" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="C30" s="2" t="s">
+      <c r="D30" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="D30" s="2" t="s">
-        <v>8</v>
-      </c>
       <c r="E30" s="2" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
     </row>
     <row r="31" spans="1:5" ht="30.75">
@@ -1840,11 +1835,11 @@
       <c r="C31" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="D31" s="2" t="s">
-        <v>8</v>
+      <c r="D31" s="1" t="s">
+        <v>82</v>
       </c>
       <c r="E31" s="2" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
     </row>
     <row r="32" spans="1:5" ht="45.75">
@@ -1857,11 +1852,11 @@
       <c r="C32" s="2" t="s">
         <v>88</v>
       </c>
-      <c r="D32" s="2" t="s">
-        <v>8</v>
+      <c r="D32" s="1" t="s">
+        <v>82</v>
       </c>
       <c r="E32" s="2" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
     </row>
     <row r="33" spans="1:5" ht="30.75">
@@ -1878,7 +1873,7 @@
         <v>13</v>
       </c>
       <c r="E33" s="2" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
     </row>
     <row r="34" spans="1:5" ht="30.75">
@@ -1895,7 +1890,7 @@
         <v>17</v>
       </c>
       <c r="E34" s="2" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
     </row>
     <row r="35" spans="1:5" ht="30.75">
@@ -1912,7 +1907,7 @@
         <v>17</v>
       </c>
       <c r="E35" s="2" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
     </row>
     <row r="36" spans="1:5" ht="30.75">
@@ -1929,7 +1924,7 @@
         <v>17</v>
       </c>
       <c r="E36" s="2" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
     </row>
     <row r="37" spans="1:5" ht="30.75">
@@ -1946,7 +1941,7 @@
         <v>17</v>
       </c>
       <c r="E37" s="2" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
     </row>
     <row r="38" spans="1:5" ht="30.75">
@@ -1963,7 +1958,7 @@
         <v>17</v>
       </c>
       <c r="E38" s="2" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
     </row>
     <row r="39" spans="1:5" ht="45.75">
@@ -1980,7 +1975,7 @@
         <v>17</v>
       </c>
       <c r="E39" s="2" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
     </row>
     <row r="40" spans="1:5" ht="30.75">
@@ -1997,7 +1992,7 @@
         <v>13</v>
       </c>
       <c r="E40" s="2" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
     </row>
     <row r="41" spans="1:5" ht="30.75">
@@ -2014,7 +2009,7 @@
         <v>13</v>
       </c>
       <c r="E41" s="2" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
     </row>
     <row r="42" spans="1:5" ht="30.75">
@@ -2031,7 +2026,7 @@
         <v>13</v>
       </c>
       <c r="E42" s="2" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
     </row>
     <row r="43" spans="1:5" ht="30.75">
@@ -2048,7 +2043,7 @@
         <v>13</v>
       </c>
       <c r="E43" s="2" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
     </row>
     <row r="44" spans="1:5" ht="30.75">
@@ -2062,10 +2057,10 @@
         <v>124</v>
       </c>
       <c r="D44" s="1" t="s">
-        <v>125</v>
+        <v>82</v>
       </c>
       <c r="E44" s="2" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
     </row>
     <row r="45" spans="1:5" ht="60.75">
@@ -2082,58 +2077,58 @@
         <v>17</v>
       </c>
       <c r="E45" s="2" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
     </row>
     <row r="46" spans="1:5" ht="45.75">
       <c r="A46" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="B46" s="2" t="s">
         <v>126</v>
       </c>
-      <c r="B46" s="2" t="s">
+      <c r="C46" s="3" t="s">
         <v>127</v>
       </c>
-      <c r="C46" s="3" t="s">
+      <c r="D46" s="2" t="s">
         <v>128</v>
       </c>
-      <c r="D46" s="2" t="s">
-        <v>129</v>
-      </c>
       <c r="E46" s="1" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
     </row>
     <row r="47" spans="1:5" ht="76.5">
       <c r="A47" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="B47" s="2" t="s">
         <v>130</v>
       </c>
-      <c r="B47" s="2" t="s">
+      <c r="C47" s="3" t="s">
         <v>131</v>
       </c>
-      <c r="C47" s="3" t="s">
-        <v>132</v>
-      </c>
-      <c r="D47" s="2" t="s">
-        <v>47</v>
+      <c r="D47" s="1" t="s">
+        <v>82</v>
       </c>
       <c r="E47" s="1" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
     </row>
     <row r="48" spans="1:5" ht="60.75">
       <c r="A48" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="B48" s="2" t="s">
         <v>133</v>
       </c>
-      <c r="B48" s="2" t="s">
+      <c r="C48" s="3" t="s">
         <v>134</v>
       </c>
-      <c r="C48" s="3" t="s">
-        <v>135</v>
-      </c>
       <c r="D48" s="1" t="s">
-        <v>136</v>
+        <v>82</v>
       </c>
       <c r="E48" s="1" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
     </row>
     <row r="49" spans="1:5">
@@ -2150,24 +2145,24 @@
         <v>55</v>
       </c>
       <c r="E49" s="2" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
     </row>
     <row r="50" spans="1:5" ht="45.75">
       <c r="A50" s="2" t="s">
+        <v>136</v>
+      </c>
+      <c r="B50" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="C50" s="3" t="s">
         <v>138</v>
       </c>
-      <c r="B50" s="2" t="s">
+      <c r="D50" s="1" t="s">
         <v>139</v>
       </c>
-      <c r="C50" s="3" t="s">
+      <c r="E50" s="1" t="s">
         <v>140</v>
-      </c>
-      <c r="D50" s="1" t="s">
-        <v>141</v>
-      </c>
-      <c r="E50" s="1" t="s">
-        <v>142</v>
       </c>
     </row>
   </sheetData>
@@ -2211,6 +2206,38 @@
     <hyperlink ref="C45" r:id="rId34" xr:uid="{397F1BF4-4E90-4516-B5E6-F02C14DD6256}"/>
     <hyperlink ref="C50" r:id="rId35" location="/" xr:uid="{148ABF7C-1E6C-4BDD-B1E3-DC7183537F2D}"/>
   </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{44AD1A21-A9D9-4471-A4AB-37CC6BEBE749}">
+  <dimension ref="A1:E1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:E1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:5" ht="30.75">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>